<commit_message>
del some words in xlsx
</commit_message>
<xml_diff>
--- a/KPMCHINA_IP5-top20_201712.xlsx
+++ b/KPMCHINA_IP5-top20_201712.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="120">
   <si>
     <t>NO．</t>
   </si>
@@ -46,9 +46,6 @@
     <t>http://www.cntv.cn</t>
   </si>
   <si>
-    <t>http://lianmeng.360.cn</t>
-  </si>
-  <si>
     <t>http://3m.mediav.com</t>
   </si>
   <si>
@@ -61,28 +58,10 @@
     <t>http://www.easipay.net</t>
   </si>
   <si>
-    <t>http://pinyin.sogou.com</t>
-  </si>
-  <si>
-    <t>http://cpc.sogou.com</t>
-  </si>
-  <si>
-    <t>http://popup.sohu.com</t>
-  </si>
-  <si>
-    <t>http://tv.sohu.com</t>
-  </si>
-  <si>
-    <t>http://wei.focus.cn</t>
-  </si>
-  <si>
     <t>http://khi.co.jp</t>
   </si>
   <si>
     <t>http://www.doc88.com</t>
-  </si>
-  <si>
-    <t>http://www.baike.com</t>
   </si>
   <si>
     <t>http://152.44.42</t>
@@ -123,73 +102,11 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>http://popup.sohu.com</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>http://tv.sohu.com</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>http://jieri.hdjr.org</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>http://news.chinabyte.com</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>http://www.baike.com</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>http://wei.focus.cn</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>http://sina.com.cn</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>http://afpssp.alimama.com</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>http://s.csbew.com</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>http://www.nongli114.com</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>http://a1.alicdn.com</t>
-  </si>
-  <si>
-    <t>http://omron.co.jp</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>http://jieri.hdjr.org</t>
-  </si>
-  <si>
-    <t>http://cdn.tanx.com</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>http://widget.wumii.com</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>http://www.qbaobei.com</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>http://news.chinabyte.com</t>
-  </si>
-  <si>
-    <t>http://www.chlingkong.com</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>http://www.nongli114.com</t>
@@ -912,7 +829,7 @@
   <dimension ref="A1:K116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D4" sqref="D4:K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -943,7 +860,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>0</v>
@@ -955,10 +872,10 @@
         <v>0</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -966,7 +883,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -988,7 +905,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="K2" s="1">
         <v>73</v>
@@ -1012,7 +929,7 @@
         <v>2</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="K3" s="1">
         <v>17</v>
@@ -1024,23 +941,13 @@
       <c r="C4" s="1">
         <v>3</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1">
-        <v>73</v>
-      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="1">
-        <v>3</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K4" s="1">
-        <v>11</v>
-      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1"/>
@@ -1048,23 +955,13 @@
       <c r="C5" s="1">
         <v>4</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="1">
-        <v>48</v>
-      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="1">
-        <v>4</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="1">
-        <v>11</v>
-      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1"/>
@@ -1072,23 +969,13 @@
       <c r="C6" s="1">
         <v>5</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1">
-        <v>22</v>
-      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1">
-        <v>5</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K6" s="1">
-        <v>4</v>
-      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1"/>
@@ -1096,23 +983,13 @@
       <c r="C7" s="1">
         <v>6</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="1">
-        <v>22</v>
-      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="1">
-        <v>6</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K7" s="1">
-        <v>3</v>
-      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="1"/>
@@ -1120,23 +997,13 @@
       <c r="C8" s="1">
         <v>7</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="1">
-        <v>17</v>
-      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="1">
-        <v>7</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K8" s="1">
-        <v>3</v>
-      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="1"/>
@@ -1144,23 +1011,13 @@
       <c r="C9" s="1">
         <v>8</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="1">
-        <v>16</v>
-      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="1">
-        <v>8</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K9" s="1">
-        <v>3</v>
-      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="1"/>
@@ -1168,23 +1025,13 @@
       <c r="C10" s="1">
         <v>9</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="1">
-        <v>11</v>
-      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1">
-        <v>9</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K10" s="1">
-        <v>2</v>
-      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="1"/>
@@ -1192,23 +1039,13 @@
       <c r="C11" s="1">
         <v>10</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="1">
-        <v>11</v>
-      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="1">
-        <v>10</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K11" s="1">
-        <v>2</v>
-      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="1"/>
@@ -1216,23 +1053,13 @@
       <c r="C12" s="1">
         <v>11</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="1">
-        <v>11</v>
-      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="1">
-        <v>11</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K12" s="1">
-        <v>2</v>
-      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="1"/>
@@ -1240,23 +1067,13 @@
       <c r="C13" s="1">
         <v>12</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="1">
-        <v>7</v>
-      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="1">
-        <v>12</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K13" s="1">
-        <v>2</v>
-      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="1"/>
@@ -1264,23 +1081,13 @@
       <c r="C14" s="1">
         <v>13</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="1">
-        <v>5</v>
-      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-      <c r="I14" s="1">
-        <v>13</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K14" s="1">
-        <v>2</v>
-      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="1"/>
@@ -1288,23 +1095,13 @@
       <c r="C15" s="1">
         <v>14</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="1">
-        <v>4</v>
-      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="I15" s="1">
-        <v>14</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K15" s="1">
-        <v>2</v>
-      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="1"/>
@@ -1312,23 +1109,13 @@
       <c r="C16" s="1">
         <v>15</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="1">
-        <v>3</v>
-      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="1">
-        <v>15</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K16" s="1">
-        <v>1</v>
-      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="1"/>
@@ -1336,23 +1123,13 @@
       <c r="C17" s="1">
         <v>16</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="1">
-        <v>3</v>
-      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="1">
-        <v>16</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K17" s="1">
-        <v>1</v>
-      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="1"/>
@@ -1360,23 +1137,13 @@
       <c r="C18" s="1">
         <v>17</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="1">
-        <v>3</v>
-      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="1">
-        <v>17</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="K18" s="1">
-        <v>1</v>
-      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="1"/>
@@ -1384,17 +1151,11 @@
       <c r="C19" s="1">
         <v>18</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="1">
-        <v>3</v>
-      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="1">
-        <v>18</v>
-      </c>
+      <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
@@ -1405,7 +1166,7 @@
         <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="E20" s="1">
         <v>2</v>
@@ -1425,7 +1186,7 @@
         <v>20</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="E21" s="1">
         <v>2</v>
@@ -1452,7 +1213,7 @@
         <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>0</v>
@@ -1464,10 +1225,10 @@
         <v>0</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1475,13 +1236,13 @@
         <v>2</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="C25" s="1">
         <v>1</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="E25" s="1">
         <v>54</v>
@@ -1497,7 +1258,7 @@
         <v>1</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="K25" s="1">
         <v>54</v>
@@ -1510,7 +1271,7 @@
         <v>2</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="E26" s="1">
         <v>35</v>
@@ -1521,7 +1282,7 @@
         <v>2</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="K26" s="1">
         <v>35</v>
@@ -1534,7 +1295,7 @@
         <v>3</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="E27" s="1">
         <v>30</v>
@@ -1545,7 +1306,7 @@
         <v>3</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="K27" s="1">
         <v>30</v>
@@ -1558,7 +1319,7 @@
         <v>4</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="E28" s="1">
         <v>28</v>
@@ -1569,7 +1330,7 @@
         <v>4</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="K28" s="1">
         <v>28</v>
@@ -1593,7 +1354,7 @@
         <v>5</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="K29" s="1">
         <v>23</v>
@@ -1606,7 +1367,7 @@
         <v>6</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="E30" s="1">
         <v>23</v>
@@ -1617,7 +1378,7 @@
         <v>6</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="K30" s="1">
         <v>23</v>
@@ -1630,7 +1391,7 @@
         <v>7</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="E31" s="1">
         <v>22</v>
@@ -1641,7 +1402,7 @@
         <v>7</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="K31" s="1">
         <v>22</v>
@@ -1654,7 +1415,7 @@
         <v>8</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E32" s="1">
         <v>21</v>
@@ -1665,7 +1426,7 @@
         <v>8</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="K32" s="1">
         <v>21</v>
@@ -1678,7 +1439,7 @@
         <v>9</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="E33" s="1">
         <v>21</v>
@@ -1689,7 +1450,7 @@
         <v>9</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="K33" s="1">
         <v>21</v>
@@ -1702,7 +1463,7 @@
         <v>10</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E34" s="1">
         <v>19</v>
@@ -1713,7 +1474,7 @@
         <v>10</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="K34" s="1">
         <v>19</v>
@@ -1726,7 +1487,7 @@
         <v>11</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="E35" s="1">
         <v>17</v>
@@ -1737,7 +1498,7 @@
         <v>11</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="K35" s="1">
         <v>17</v>
@@ -1750,7 +1511,7 @@
         <v>12</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="E36" s="1">
         <v>16</v>
@@ -1761,7 +1522,7 @@
         <v>12</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="K36" s="1">
         <v>16</v>
@@ -1774,7 +1535,7 @@
         <v>13</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="E37" s="1">
         <v>13</v>
@@ -1785,7 +1546,7 @@
         <v>13</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="K37" s="1">
         <v>13</v>
@@ -1798,7 +1559,7 @@
         <v>14</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="E38" s="1">
         <v>12</v>
@@ -1809,7 +1570,7 @@
         <v>14</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="K38" s="1">
         <v>12</v>
@@ -1822,7 +1583,7 @@
         <v>15</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E39" s="1">
         <v>12</v>
@@ -1833,7 +1594,7 @@
         <v>15</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K39" s="1">
         <v>12</v>
@@ -1846,7 +1607,7 @@
         <v>16</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="E40" s="1">
         <v>12</v>
@@ -1857,7 +1618,7 @@
         <v>16</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="K40" s="1">
         <v>12</v>
@@ -1870,7 +1631,7 @@
         <v>17</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="E41" s="1">
         <v>10</v>
@@ -1881,7 +1642,7 @@
         <v>17</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="K41" s="1">
         <v>10</v>
@@ -1894,7 +1655,7 @@
         <v>18</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="E42" s="1">
         <v>8</v>
@@ -1905,7 +1666,7 @@
         <v>18</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="K42" s="1">
         <v>8</v>
@@ -1918,7 +1679,7 @@
         <v>19</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E43" s="1">
         <v>6</v>
@@ -1929,7 +1690,7 @@
         <v>19</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K43" s="1">
         <v>6</v>
@@ -1942,7 +1703,7 @@
         <v>20</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E44" s="1">
         <v>6</v>
@@ -1953,7 +1714,7 @@
         <v>20</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K44" s="1">
         <v>6</v>
@@ -1973,7 +1734,7 @@
         <v>2</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>0</v>
@@ -1985,10 +1746,10 @@
         <v>0</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -1996,13 +1757,13 @@
         <v>3</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="C51" s="1">
         <v>1</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E51" s="1">
         <v>342</v>
@@ -2018,7 +1779,7 @@
         <v>1</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="K51" s="1">
         <v>317</v>
@@ -2042,7 +1803,7 @@
         <v>2</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="K52" s="1">
         <v>14</v>
@@ -2055,7 +1816,7 @@
         <v>3</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="E53" s="1">
         <v>1</v>
@@ -2066,7 +1827,7 @@
         <v>3</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="K53" s="1">
         <v>1</v>
@@ -2079,7 +1840,7 @@
         <v>4</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="E54" s="1">
         <v>1</v>
@@ -2090,7 +1851,7 @@
         <v>4</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="K54" s="1">
         <v>1</v>
@@ -2103,7 +1864,7 @@
         <v>5</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="E55" s="1">
         <v>1</v>
@@ -2114,7 +1875,7 @@
         <v>5</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="K55" s="1">
         <v>1</v>
@@ -2138,7 +1899,7 @@
         <v>6</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="K56" s="1">
         <v>1</v>
@@ -2151,7 +1912,7 @@
         <v>7</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="E57" s="1">
         <v>1</v>
@@ -2162,7 +1923,7 @@
         <v>7</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="K57" s="1">
         <v>1</v>
@@ -2390,7 +2151,7 @@
         <v>2</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>0</v>
@@ -2402,10 +2163,10 @@
         <v>0</v>
       </c>
       <c r="J73" s="2" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
     </row>
     <row r="74" spans="1:11">
@@ -2413,13 +2174,13 @@
         <v>4</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="C74" s="1">
         <v>1</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="E74" s="1">
         <v>55</v>
@@ -2435,7 +2196,7 @@
         <v>1</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="K74" s="1">
         <v>55</v>
@@ -2448,7 +2209,7 @@
         <v>2</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E75" s="1">
         <v>37</v>
@@ -2459,7 +2220,7 @@
         <v>2</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="K75" s="1">
         <v>37</v>
@@ -2483,7 +2244,7 @@
         <v>3</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="K76" s="1">
         <v>27</v>
@@ -2496,7 +2257,7 @@
         <v>4</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="E77" s="1">
         <v>20</v>
@@ -2507,7 +2268,7 @@
         <v>4</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="K77" s="1">
         <v>20</v>
@@ -2520,7 +2281,7 @@
         <v>5</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="E78" s="1">
         <v>14</v>
@@ -2531,7 +2292,7 @@
         <v>5</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="K78" s="1">
         <v>14</v>
@@ -2544,7 +2305,7 @@
         <v>6</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="E79" s="1">
         <v>14</v>
@@ -2555,7 +2316,7 @@
         <v>6</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="K79" s="1">
         <v>14</v>
@@ -2579,7 +2340,7 @@
         <v>7</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="K80" s="1">
         <v>14</v>
@@ -2603,7 +2364,7 @@
         <v>8</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="K81" s="1">
         <v>14</v>
@@ -2616,7 +2377,7 @@
         <v>9</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="E82" s="1">
         <v>11</v>
@@ -2627,7 +2388,7 @@
         <v>9</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="K82" s="1">
         <v>11</v>
@@ -2640,7 +2401,7 @@
         <v>10</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="E83" s="1">
         <v>10</v>
@@ -2651,7 +2412,7 @@
         <v>10</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="K83" s="1">
         <v>10</v>
@@ -2664,7 +2425,7 @@
         <v>11</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="E84" s="1">
         <v>10</v>
@@ -2675,7 +2436,7 @@
         <v>11</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
       <c r="K84" s="1">
         <v>10</v>
@@ -2699,7 +2460,7 @@
         <v>12</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="K85" s="1">
         <v>8</v>
@@ -2712,7 +2473,7 @@
         <v>13</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="E86" s="1">
         <v>8</v>
@@ -2723,7 +2484,7 @@
         <v>13</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="K86" s="1">
         <v>8</v>
@@ -2736,7 +2497,7 @@
         <v>14</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="E87" s="1">
         <v>8</v>
@@ -2747,7 +2508,7 @@
         <v>14</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="K87" s="1">
         <v>8</v>
@@ -2760,7 +2521,7 @@
         <v>15</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="E88" s="1">
         <v>7</v>
@@ -2771,7 +2532,7 @@
         <v>15</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="K88" s="1">
         <v>7</v>
@@ -2784,7 +2545,7 @@
         <v>16</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="E89" s="1">
         <v>5</v>
@@ -2795,7 +2556,7 @@
         <v>16</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="K89" s="1">
         <v>5</v>
@@ -2808,7 +2569,7 @@
         <v>17</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="E90" s="1">
         <v>5</v>
@@ -2819,7 +2580,7 @@
         <v>17</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="K90" s="1">
         <v>5</v>
@@ -2832,7 +2593,7 @@
         <v>18</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="E91" s="1">
         <v>5</v>
@@ -2843,7 +2604,7 @@
         <v>18</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="K91" s="1">
         <v>5</v>
@@ -2856,7 +2617,7 @@
         <v>19</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="E92" s="1">
         <v>4</v>
@@ -2867,7 +2628,7 @@
         <v>19</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="K92" s="1">
         <v>4</v>
@@ -2880,7 +2641,7 @@
         <v>20</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E93" s="1">
         <v>4</v>
@@ -2891,7 +2652,7 @@
         <v>20</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="K93" s="1">
         <v>4</v>
@@ -2911,7 +2672,7 @@
         <v>2</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="G96" s="2" t="s">
         <v>0</v>
@@ -2923,10 +2684,10 @@
         <v>0</v>
       </c>
       <c r="J96" s="2" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="K96" s="2" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
     </row>
     <row r="97" spans="1:11">
@@ -2934,13 +2695,13 @@
         <v>5</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C97" s="1">
         <v>1</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E97" s="1">
         <v>130</v>
@@ -2956,7 +2717,7 @@
         <v>1</v>
       </c>
       <c r="J97" s="1" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="K97" s="1">
         <v>130</v>
@@ -2969,7 +2730,7 @@
         <v>2</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E98" s="1">
         <v>120</v>
@@ -2980,7 +2741,7 @@
         <v>2</v>
       </c>
       <c r="J98" s="1" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="K98" s="1">
         <v>120</v>
@@ -2993,7 +2754,7 @@
         <v>3</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E99" s="1">
         <v>24</v>
@@ -3004,7 +2765,7 @@
         <v>3</v>
       </c>
       <c r="J99" s="1" t="s">
-        <v>135</v>
+        <v>112</v>
       </c>
       <c r="K99" s="1">
         <v>24</v>
@@ -3017,7 +2778,7 @@
         <v>4</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E100" s="1">
         <v>8</v>
@@ -3028,7 +2789,7 @@
         <v>4</v>
       </c>
       <c r="J100" s="1" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="K100" s="1">
         <v>8</v>
@@ -3041,7 +2802,7 @@
         <v>5</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E101" s="1">
         <v>4</v>
@@ -3052,7 +2813,7 @@
         <v>5</v>
       </c>
       <c r="J101" s="1" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="K101" s="1">
         <v>4</v>
@@ -3065,7 +2826,7 @@
         <v>6</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E102" s="1">
         <v>3</v>
@@ -3076,7 +2837,7 @@
         <v>6</v>
       </c>
       <c r="J102" s="1" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="K102" s="1">
         <v>3</v>
@@ -3089,7 +2850,7 @@
         <v>7</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
       <c r="E103" s="1">
         <v>3</v>
@@ -3100,7 +2861,7 @@
         <v>7</v>
       </c>
       <c r="J103" s="1" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="K103" s="1">
         <v>3</v>
@@ -3113,7 +2874,7 @@
         <v>8</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>141</v>
+        <v>118</v>
       </c>
       <c r="E104" s="1">
         <v>1</v>
@@ -3124,7 +2885,7 @@
         <v>8</v>
       </c>
       <c r="J104" s="1" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="K104" s="1">
         <v>1</v>

</xml_diff>